<commit_message>
new files 21 october
</commit_message>
<xml_diff>
--- a/Evaluation_Results/Final_TestFiles_2ndOctober_FewShotTest_Embeddings/detailed_category_results_GPT5_5_shot.xlsx
+++ b/Evaluation_Results/Final_TestFiles_2ndOctober_FewShotTest_Embeddings/detailed_category_results_GPT5_5_shot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,6 +711,192 @@
         <v>108</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10/03/2025</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GPT5</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Crop</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>77</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>77</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>77</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10/03/2025</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GPT5</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>46</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>46</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>46</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>10/03/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GPT5</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TimeStatement</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>108</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>108</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>108</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>